<commit_message>
-Agregando el documento de la tesis -Modificando pequeños detalles en el código
</commit_message>
<xml_diff>
--- a/Experimentos.xlsx
+++ b/Experimentos.xlsx
@@ -778,32 +778,32 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="inlineStr">
+      <c r="A1" s="11" t="inlineStr">
         <is>
           <t>Model</t>
         </is>
       </c>
-      <c r="B1" s="4" t="inlineStr">
+      <c r="B1" s="11" t="inlineStr">
         <is>
           <t>Accuracy</t>
         </is>
       </c>
-      <c r="C1" s="4" t="inlineStr">
+      <c r="C1" s="11" t="inlineStr">
         <is>
           <t>AUC</t>
         </is>
       </c>
-      <c r="D1" s="4" t="inlineStr">
+      <c r="D1" s="11" t="inlineStr">
         <is>
           <t>Precision Score</t>
         </is>
       </c>
-      <c r="E1" s="4" t="inlineStr">
+      <c r="E1" s="11" t="inlineStr">
         <is>
           <t>Recall Score</t>
         </is>
       </c>
-      <c r="F1" s="4" t="inlineStr">
+      <c r="F1" s="11" t="inlineStr">
         <is>
           <t>F1 Score</t>
         </is>
@@ -813,92 +813,92 @@
     <row r="2">
       <c r="A2" s="10" t="inlineStr">
         <is>
-          <t>RF IMABALANCED</t>
+          <t>RF OVERSAMPLE</t>
         </is>
       </c>
       <c r="B2" s="10" t="n">
         <v>0.99775</v>
       </c>
       <c r="C2" s="10" t="n">
-        <v>0.6815674924223434</v>
+        <v>0.625</v>
       </c>
       <c r="D2" s="10" t="n">
-        <v>0.6666666666666666</v>
+        <v>1</v>
       </c>
       <c r="E2" s="10" t="n">
-        <v>0.3636363636363636</v>
+        <v>0.25</v>
       </c>
       <c r="F2" s="10" t="n">
-        <v>0.4705882352941177</v>
+        <v>0.4</v>
       </c>
       <c r="G2" s="10" t="n"/>
     </row>
     <row r="3">
       <c r="A3" s="10" t="inlineStr">
         <is>
-          <t>XGBOOST IMBALANCED</t>
+          <t>RF SMOTE</t>
         </is>
       </c>
       <c r="B3" s="10" t="n">
-        <v>0.9975000000000001</v>
+        <v>0.996</v>
       </c>
       <c r="C3" s="10" t="n">
-        <v>0.681442147724424</v>
+        <v>0.6313277542008752</v>
       </c>
       <c r="D3" s="10" t="n">
-        <v>0.5714285714285714</v>
+        <v>0.7142857142857143</v>
       </c>
       <c r="E3" s="10" t="n">
-        <v>0.3636363636363636</v>
+        <v>0.2631578947368421</v>
       </c>
       <c r="F3" s="10" t="n">
-        <v>0.4444444444444444</v>
+        <v>0.3846153846153846</v>
       </c>
       <c r="G3" s="10" t="n"/>
     </row>
     <row r="4">
       <c r="A4" s="10" t="inlineStr">
         <is>
-          <t>KNN IMBALANCE</t>
+          <t>RF IMABALANCED</t>
         </is>
       </c>
       <c r="B4" s="10" t="n">
-        <v>0.99775</v>
+        <v>0.99675</v>
       </c>
       <c r="C4" s="10" t="n">
-        <v>0.5909090909090909</v>
+        <v>0.5998745294855709</v>
       </c>
       <c r="D4" s="10" t="n">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="E4" s="10" t="n">
-        <v>0.1818181818181818</v>
+        <v>0.2</v>
       </c>
       <c r="F4" s="10" t="n">
-        <v>0.3076923076923077</v>
+        <v>0.3157894736842106</v>
       </c>
       <c r="G4" s="10" t="n"/>
     </row>
     <row r="5">
       <c r="A5" s="10" t="inlineStr">
         <is>
-          <t>DT IMBALANCED</t>
+          <t>XGBOOST IMBALANCED</t>
         </is>
       </c>
       <c r="B5" s="10" t="n">
-        <v>0.99425</v>
+        <v>0.99675</v>
       </c>
       <c r="C5" s="10" t="n">
-        <v>0.6798126666514734</v>
+        <v>0.5998745294855709</v>
       </c>
       <c r="D5" s="10" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="E5" s="10" t="n">
         <v>0.2</v>
       </c>
-      <c r="E5" s="10" t="n">
-        <v>0.3636363636363636</v>
-      </c>
       <c r="F5" s="10" t="n">
-        <v>0.2580645161290323</v>
+        <v>0.3157894736842106</v>
       </c>
       <c r="G5" s="10" t="n"/>
     </row>
@@ -909,272 +909,272 @@
         </is>
       </c>
       <c r="B6" s="10" t="n">
-        <v>0.997</v>
+        <v>0.996</v>
       </c>
       <c r="C6" s="10" t="n">
-        <v>0.5830825810765631</v>
+        <v>0.5832077682906412</v>
       </c>
       <c r="D6" s="10" t="n">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="E6" s="10" t="n">
         <v>0.1666666666666667</v>
       </c>
       <c r="F6" s="10" t="n">
-        <v>0.25</v>
+        <v>0.2727272727272728</v>
       </c>
       <c r="G6" s="10" t="n"/>
     </row>
     <row r="7">
       <c r="A7" s="10" t="inlineStr">
         <is>
-          <t>RF OVERSAMPLE</t>
+          <t>XGBOOST OVERSAMPLE</t>
         </is>
       </c>
       <c r="B7" s="10" t="n">
-        <v>0.997</v>
+        <v>0.996</v>
       </c>
       <c r="C7" s="10" t="n">
-        <v>0.5994987468671679</v>
+        <v>0.624122367101304</v>
       </c>
       <c r="D7" s="10" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.3</v>
       </c>
       <c r="E7" s="10" t="n">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="F7" s="10" t="n">
-        <v>0.25</v>
+        <v>0.2727272727272727</v>
       </c>
       <c r="G7" s="10" t="n"/>
     </row>
     <row r="8">
       <c r="A8" s="10" t="inlineStr">
         <is>
-          <t>XGBOOST OVERSAMPLE</t>
+          <t xml:space="preserve">XGBOOST ADASYN </t>
         </is>
       </c>
       <c r="B8" s="10" t="n">
-        <v>0.9965000000000001</v>
+        <v>0.99325</v>
       </c>
       <c r="C8" s="10" t="n">
-        <v>0.5992481203007519</v>
+        <v>0.6371309782911992</v>
       </c>
       <c r="D8" s="10" t="n">
-        <v>0.25</v>
+        <v>0.2631578947368421</v>
       </c>
       <c r="E8" s="10" t="n">
-        <v>0.2</v>
+        <v>0.2777777777777778</v>
       </c>
       <c r="F8" s="10" t="n">
-        <v>0.2222222222222222</v>
+        <v>0.2702702702702702</v>
       </c>
       <c r="G8" s="10" t="n"/>
     </row>
     <row r="9">
       <c r="A9" s="10" t="inlineStr">
         <is>
-          <t>DT OVERSAMPLE</t>
+          <t>XGBOOST SMOTE</t>
         </is>
       </c>
       <c r="B9" s="10" t="n">
-        <v>0.99575</v>
+        <v>0.9925</v>
       </c>
       <c r="C9" s="10" t="n">
-        <v>0.5988721804511278</v>
+        <v>0.6295694020280543</v>
       </c>
       <c r="D9" s="10" t="n">
-        <v>0.1818181818181818</v>
+        <v>0.2380952380952381</v>
       </c>
       <c r="E9" s="10" t="n">
-        <v>0.2</v>
+        <v>0.2631578947368421</v>
       </c>
       <c r="F9" s="10" t="n">
-        <v>0.1904761904761905</v>
+        <v>0.25</v>
       </c>
       <c r="G9" s="10" t="n"/>
     </row>
     <row r="10">
       <c r="A10" s="10" t="inlineStr">
         <is>
-          <t>RF SMOTE</t>
+          <t>KNN IMBALANCE</t>
         </is>
       </c>
       <c r="B10" s="10" t="n">
         <v>0.99675</v>
       </c>
       <c r="C10" s="10" t="n">
-        <v>0.5357142857142857</v>
+        <v>0.5666666666666667</v>
       </c>
       <c r="D10" s="10" t="n">
         <v>1</v>
       </c>
       <c r="E10" s="10" t="n">
-        <v>0.07142857142857142</v>
+        <v>0.1333333333333333</v>
       </c>
       <c r="F10" s="10" t="n">
-        <v>0.1333333333333333</v>
+        <v>0.2352941176470588</v>
       </c>
       <c r="G10" s="10" t="n"/>
     </row>
     <row r="11">
       <c r="A11" s="10" t="inlineStr">
         <is>
-          <t xml:space="preserve">XGBOOST ADASYN </t>
+          <t>DT IMBALANCED</t>
         </is>
       </c>
       <c r="B11" s="10" t="n">
-        <v>0.9925</v>
+        <v>0.995</v>
       </c>
       <c r="C11" s="10" t="n">
-        <v>0.5808258107656303</v>
+        <v>0.5989962358845672</v>
       </c>
       <c r="D11" s="10" t="n">
-        <v>0.09090909090909091</v>
+        <v>0.2727272727272727</v>
       </c>
       <c r="E11" s="10" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.2</v>
       </c>
       <c r="F11" s="10" t="n">
-        <v>0.1176470588235294</v>
+        <v>0.2307692307692308</v>
       </c>
       <c r="G11" s="10" t="n"/>
     </row>
     <row r="12">
       <c r="A12" s="10" t="inlineStr">
         <is>
-          <t>NB IMBALANCED</t>
+          <t>DT OVERSAMPLE</t>
         </is>
       </c>
       <c r="B12" s="10" t="n">
-        <v>0.98</v>
+        <v>0.99575</v>
       </c>
       <c r="C12" s="10" t="n">
-        <v>0.7179972196267007</v>
+        <v>0.5824557004346373</v>
       </c>
       <c r="D12" s="10" t="n">
-        <v>0.06329113924050633</v>
+        <v>0.2222222222222222</v>
       </c>
       <c r="E12" s="10" t="n">
-        <v>0.4545454545454545</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="F12" s="10" t="n">
-        <v>0.1111111111111111</v>
+        <v>0.1904761904761905</v>
       </c>
       <c r="G12" s="10" t="n"/>
     </row>
     <row r="13">
       <c r="A13" s="10" t="inlineStr">
         <is>
-          <t>XGBOOST SMOTE</t>
+          <t>NB SMOTE</t>
         </is>
       </c>
       <c r="B13" s="10" t="n">
-        <v>0.99425</v>
+        <v>0.97525</v>
       </c>
       <c r="C13" s="10" t="n">
-        <v>0.5344598953480036</v>
+        <v>0.6994738164174565</v>
       </c>
       <c r="D13" s="10" t="n">
-        <v>0.09090909090909091</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="E13" s="10" t="n">
-        <v>0.07142857142857142</v>
+        <v>0.4210526315789473</v>
       </c>
       <c r="F13" s="10" t="n">
-        <v>0.08</v>
+        <v>0.1391304347826087</v>
       </c>
       <c r="G13" s="10" t="n"/>
     </row>
     <row r="14">
       <c r="A14" s="10" t="inlineStr">
         <is>
-          <t xml:space="preserve">LR ADASYN </t>
+          <t>DT SMOTE</t>
         </is>
       </c>
       <c r="B14" s="10" t="n">
-        <v>0.986</v>
+        <v>0.98525</v>
       </c>
       <c r="C14" s="10" t="n">
-        <v>0.5775660314276162</v>
+        <v>0.5997369082087283</v>
       </c>
       <c r="D14" s="10" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="E14" s="10" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.2105263157894737</v>
       </c>
       <c r="F14" s="10" t="n">
-        <v>0.06666666666666667</v>
+        <v>0.1194029850746269</v>
       </c>
       <c r="G14" s="10" t="n"/>
     </row>
     <row r="15">
       <c r="A15" s="10" t="inlineStr">
         <is>
-          <t>NB UNDERSAMPLE</t>
+          <t>LR SMOTE</t>
         </is>
       </c>
       <c r="B15" s="10" t="n">
-        <v>0.9642500000000001</v>
+        <v>0.987</v>
       </c>
       <c r="C15" s="10" t="n">
-        <v>0.7101005036577862</v>
+        <v>0.5744258914052275</v>
       </c>
       <c r="D15" s="10" t="n">
-        <v>0.0352112676056338</v>
+        <v>0.07692307692307693</v>
       </c>
       <c r="E15" s="10" t="n">
-        <v>0.4545454545454545</v>
+        <v>0.1578947368421053</v>
       </c>
       <c r="F15" s="10" t="n">
-        <v>0.06535947712418301</v>
+        <v>0.103448275862069</v>
       </c>
       <c r="G15" s="10" t="n"/>
     </row>
     <row r="16">
       <c r="A16" s="10" t="inlineStr">
         <is>
-          <t>LR SMOTE</t>
+          <t>KNN OVERSAMPLE</t>
         </is>
       </c>
       <c r="B16" s="10" t="n">
-        <v>0.98525</v>
+        <v>0.991</v>
       </c>
       <c r="C16" s="10" t="n">
-        <v>0.5655329367070461</v>
+        <v>0.5800735539953193</v>
       </c>
       <c r="D16" s="10" t="n">
-        <v>0.04081632653061224</v>
+        <v>0.07142857142857142</v>
       </c>
       <c r="E16" s="10" t="n">
-        <v>0.1428571428571428</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="F16" s="10" t="n">
-        <v>0.06349206349206349</v>
+        <v>0.1</v>
       </c>
       <c r="G16" s="10" t="n"/>
     </row>
     <row r="17">
       <c r="A17" s="10" t="inlineStr">
         <is>
-          <t>LR OVERSAMPLE</t>
+          <t>NB IMBALANCED</t>
         </is>
       </c>
       <c r="B17" s="10" t="n">
-        <v>0.9845</v>
+        <v>0.9785</v>
       </c>
       <c r="C17" s="10" t="n">
-        <v>0.5932330827067669</v>
+        <v>0.6239230447511501</v>
       </c>
       <c r="D17" s="10" t="n">
-        <v>0.03571428571428571</v>
+        <v>0.05063291139240506</v>
       </c>
       <c r="E17" s="10" t="n">
-        <v>0.2</v>
+        <v>0.2666666666666667</v>
       </c>
       <c r="F17" s="10" t="n">
-        <v>0.06060606060606061</v>
+        <v>0.0851063829787234</v>
       </c>
       <c r="G17" s="10" t="n"/>
     </row>
@@ -1185,249 +1185,249 @@
         </is>
       </c>
       <c r="B18" s="10" t="n">
-        <v>0.969</v>
+        <v>0.96475</v>
       </c>
       <c r="C18" s="10" t="n">
-        <v>0.6105817452357071</v>
+        <v>0.6504687761593838</v>
       </c>
       <c r="D18" s="10" t="n">
-        <v>0.02542372881355932</v>
+        <v>0.04444444444444445</v>
       </c>
       <c r="E18" s="10" t="n">
-        <v>0.25</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="F18" s="10" t="n">
-        <v>0.04615384615384616</v>
+        <v>0.07843137254901961</v>
       </c>
       <c r="G18" s="10" t="n"/>
     </row>
     <row r="19">
       <c r="A19" s="10" t="inlineStr">
         <is>
-          <t>DT SMOTE</t>
+          <t>LR OVERSAMPLE</t>
         </is>
       </c>
       <c r="B19" s="10" t="n">
-        <v>0.98575</v>
+        <v>0.982</v>
       </c>
       <c r="C19" s="10" t="n">
-        <v>0.5301949681026449</v>
+        <v>0.6171013039117352</v>
       </c>
       <c r="D19" s="10" t="n">
-        <v>0.02222222222222222</v>
+        <v>0.04545454545454546</v>
       </c>
       <c r="E19" s="10" t="n">
-        <v>0.07142857142857142</v>
+        <v>0.25</v>
       </c>
       <c r="F19" s="10" t="n">
-        <v>0.03389830508474576</v>
+        <v>0.07692307692307693</v>
       </c>
       <c r="G19" s="10" t="n"/>
     </row>
     <row r="20">
       <c r="A20" s="10" t="inlineStr">
         <is>
-          <t>MLPClassifier  ADASYN</t>
+          <t xml:space="preserve">LR ADASYN </t>
         </is>
       </c>
       <c r="B20" s="10" t="n">
-        <v>0.95275</v>
+        <v>0.97975</v>
       </c>
       <c r="C20" s="10" t="n">
-        <v>0.602432296890672</v>
+        <v>0.5750460405156538</v>
       </c>
       <c r="D20" s="10" t="n">
-        <v>0.01639344262295082</v>
+        <v>0.04347826086956522</v>
       </c>
       <c r="E20" s="10" t="n">
-        <v>0.25</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="F20" s="10" t="n">
-        <v>0.03076923076923077</v>
+        <v>0.06896551724137931</v>
       </c>
       <c r="G20" s="10" t="n"/>
     </row>
     <row r="21">
       <c r="A21" s="10" t="inlineStr">
         <is>
-          <t>DT ADASYN</t>
+          <t>NB OVERSAMPLE</t>
         </is>
       </c>
       <c r="B21" s="10" t="n">
-        <v>0.9825</v>
+        <v>0.96575</v>
       </c>
       <c r="C21" s="10" t="n">
-        <v>0.5342694750919424</v>
+        <v>0.6504931461049815</v>
       </c>
       <c r="D21" s="10" t="n">
-        <v>0.01666666666666667</v>
+        <v>0.03007518796992481</v>
       </c>
       <c r="E21" s="10" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="F21" s="10" t="n">
-        <v>0.02777777777777778</v>
+        <v>0.05517241379310345</v>
       </c>
       <c r="G21" s="10" t="n"/>
     </row>
     <row r="22">
       <c r="A22" s="10" t="inlineStr">
         <is>
-          <t>NB OVERSAMPLE</t>
+          <t>MLPClassifier  ADASYN</t>
         </is>
       </c>
       <c r="B22" s="10" t="n">
-        <v>0.96275</v>
+        <v>0.94475</v>
       </c>
       <c r="C22" s="10" t="n">
-        <v>0.5823308270676691</v>
+        <v>0.6404235727440146</v>
       </c>
       <c r="D22" s="10" t="n">
-        <v>0.01398601398601399</v>
+        <v>0.02790697674418605</v>
       </c>
       <c r="E22" s="10" t="n">
-        <v>0.2</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="F22" s="10" t="n">
-        <v>0.0261437908496732</v>
+        <v>0.05150214592274679</v>
       </c>
       <c r="G22" s="10" t="n"/>
     </row>
     <row r="23">
       <c r="A23" s="10" t="inlineStr">
         <is>
-          <t>MLPClassifier SMOTE</t>
+          <t>NB UNDERSAMPLE</t>
         </is>
       </c>
       <c r="B23" s="10" t="n">
-        <v>0.95575</v>
+        <v>0.96125</v>
       </c>
       <c r="C23" s="10" t="n">
-        <v>0.5507311303849186</v>
+        <v>0.6152655792555416</v>
       </c>
       <c r="D23" s="10" t="n">
-        <v>0.01197604790419162</v>
+        <v>0.02702702702702703</v>
       </c>
       <c r="E23" s="10" t="n">
-        <v>0.1428571428571428</v>
+        <v>0.2666666666666667</v>
       </c>
       <c r="F23" s="10" t="n">
-        <v>0.02209944751381215</v>
+        <v>0.049079754601227</v>
       </c>
       <c r="G23" s="10" t="n"/>
     </row>
     <row r="24">
       <c r="A24" s="10" t="inlineStr">
         <is>
-          <t>NB SMOTE</t>
+          <t>DT ADASYN</t>
         </is>
       </c>
       <c r="B24" s="10" t="n">
-        <v>0.972</v>
+        <v>0.9795</v>
       </c>
       <c r="C24" s="10" t="n">
-        <v>0.523295821088094</v>
+        <v>0.5472682627378761</v>
       </c>
       <c r="D24" s="10" t="n">
-        <v>0.01</v>
+        <v>0.02941176470588235</v>
       </c>
       <c r="E24" s="10" t="n">
-        <v>0.07142857142857142</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="F24" s="10" t="n">
-        <v>0.01754385964912281</v>
+        <v>0.04651162790697674</v>
       </c>
       <c r="G24" s="10" t="n"/>
     </row>
     <row r="25">
       <c r="A25" s="10" t="inlineStr">
         <is>
-          <t>KNN SMOTE</t>
+          <t>MLPClassifier SMOTE</t>
         </is>
       </c>
       <c r="B25" s="10" t="n">
-        <v>0.76225</v>
+        <v>0.854</v>
       </c>
       <c r="C25" s="10" t="n">
-        <v>0.5959967027453229</v>
+        <v>0.7171300519573236</v>
       </c>
       <c r="D25" s="10" t="n">
-        <v>0.006322444678609062</v>
+        <v>0.01873935264054515</v>
       </c>
       <c r="E25" s="10" t="n">
-        <v>0.4285714285714285</v>
+        <v>0.5789473684210527</v>
       </c>
       <c r="F25" s="10" t="n">
-        <v>0.01246105919003115</v>
+        <v>0.03630363036303631</v>
       </c>
       <c r="G25" s="10" t="n"/>
     </row>
     <row r="26">
       <c r="A26" s="10" t="inlineStr">
         <is>
-          <t>RF UNDERSAMPLE</t>
+          <t>KNN SMOTE</t>
         </is>
       </c>
       <c r="B26" s="10" t="n">
-        <v>0.724</v>
+        <v>0.73775</v>
       </c>
       <c r="C26" s="10" t="n">
-        <v>0.6349734497139862</v>
+        <v>0.6325374476130038</v>
       </c>
       <c r="D26" s="10" t="n">
-        <v>0.005429864253393665</v>
+        <v>0.009523809523809525</v>
       </c>
       <c r="E26" s="10" t="n">
-        <v>0.5454545454545454</v>
+        <v>0.5263157894736842</v>
       </c>
       <c r="F26" s="10" t="n">
-        <v>0.01075268817204301</v>
+        <v>0.01870907390084191</v>
       </c>
       <c r="G26" s="10" t="n"/>
     </row>
     <row r="27">
       <c r="A27" s="10" t="inlineStr">
         <is>
-          <t>KNN ADASYN</t>
+          <t>DT UNDERSAMPLE</t>
         </is>
       </c>
       <c r="B27" s="10" t="n">
-        <v>0.806</v>
+        <v>0.63225</v>
       </c>
       <c r="C27" s="10" t="n">
-        <v>0.5703778000668672</v>
+        <v>0.6493935591802592</v>
       </c>
       <c r="D27" s="10" t="n">
-        <v>0.005181347150259068</v>
+        <v>0.006775067750677507</v>
       </c>
       <c r="E27" s="10" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="F27" s="10" t="n">
-        <v>0.01020408163265306</v>
+        <v>0.01341381623071764</v>
       </c>
       <c r="G27" s="10" t="n"/>
     </row>
     <row r="28">
       <c r="A28" s="10" t="inlineStr">
         <is>
-          <t>DT UNDERSAMPLE</t>
+          <t>RF UNDERSAMPLE</t>
         </is>
       </c>
       <c r="B28" s="10" t="n">
-        <v>0.586</v>
+        <v>0.657</v>
       </c>
       <c r="C28" s="10" t="n">
-        <v>0.6111123772191709</v>
+        <v>0.5289836888331242</v>
       </c>
       <c r="D28" s="10" t="n">
-        <v>0.004219409282700422</v>
+        <v>0.004382761139517896</v>
       </c>
       <c r="E28" s="10" t="n">
-        <v>0.6363636363636364</v>
+        <v>0.4</v>
       </c>
       <c r="F28" s="10" t="n">
-        <v>0.008383233532934133</v>
+        <v>0.008670520231213872</v>
       </c>
       <c r="G28" s="10" t="n"/>
     </row>
@@ -1438,19 +1438,19 @@
         </is>
       </c>
       <c r="B29" s="10" t="n">
-        <v>0.32725</v>
+        <v>0.3085</v>
       </c>
       <c r="C29" s="10" t="n">
-        <v>0.5720390163859705</v>
+        <v>0.5533249686323714</v>
       </c>
       <c r="D29" s="10" t="n">
-        <v>0.003335804299481097</v>
+        <v>0.004324324324324324</v>
       </c>
       <c r="E29" s="10" t="n">
-        <v>0.8181818181818182</v>
+        <v>0.8</v>
       </c>
       <c r="F29" s="10" t="n">
-        <v>0.006644518272425248</v>
+        <v>0.00860215053763441</v>
       </c>
       <c r="G29" s="10" t="n"/>
     </row>
@@ -1461,102 +1461,102 @@
         </is>
       </c>
       <c r="B30" s="10" t="n">
-        <v>0.57375</v>
+        <v>0.53525</v>
       </c>
       <c r="C30" s="10" t="n">
-        <v>0.5143120855078739</v>
+        <v>0.5342952739439565</v>
       </c>
       <c r="D30" s="10" t="n">
-        <v>0.002934272300469483</v>
+        <v>0.004301075268817204</v>
       </c>
       <c r="E30" s="10" t="n">
-        <v>0.4545454545454545</v>
+        <v>0.5333333333333333</v>
       </c>
       <c r="F30" s="10" t="n">
-        <v>0.005830903790087463</v>
+        <v>0.008533333333333334</v>
       </c>
       <c r="G30" s="10" t="n"/>
     </row>
     <row r="31">
       <c r="A31" s="10" t="inlineStr">
         <is>
-          <t>MLPClassifier UNDERSAMPLE</t>
+          <t>KNN ADASYN</t>
         </is>
       </c>
       <c r="B31" s="10" t="n">
-        <v>0.03425</v>
+        <v>0.759</v>
       </c>
       <c r="C31" s="10" t="n">
-        <v>0.515793431937829</v>
+        <v>0.4918243205536024</v>
       </c>
       <c r="D31" s="10" t="n">
-        <v>0.002839442436757873</v>
+        <v>0.00419287211740042</v>
       </c>
       <c r="E31" s="10" t="n">
-        <v>1</v>
+        <v>0.2222222222222222</v>
       </c>
       <c r="F31" s="10" t="n">
-        <v>0.005662805662805663</v>
+        <v>0.00823045267489712</v>
       </c>
       <c r="G31" s="10" t="n"/>
     </row>
     <row r="32">
       <c r="A32" s="10" t="inlineStr">
         <is>
-          <t>LR UNDERSAMPLE</t>
+          <t>MLPClassifier OVERSAMPLE</t>
         </is>
       </c>
       <c r="B32" s="10" t="n">
-        <v>0.00275</v>
+        <v>0.18675</v>
       </c>
       <c r="C32" s="10" t="n">
-        <v>0.5</v>
+        <v>0.5090688732865263</v>
       </c>
       <c r="D32" s="10" t="n">
-        <v>0.00275</v>
+        <v>0.00306654400490647</v>
       </c>
       <c r="E32" s="10" t="n">
-        <v>1</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="F32" s="10" t="n">
-        <v>0.005484916479680877</v>
+        <v>0.006110601894286587</v>
       </c>
       <c r="G32" s="10" t="n"/>
     </row>
     <row r="33">
       <c r="A33" s="10" t="inlineStr">
         <is>
-          <t>MLPClassifier OVERSAMPLE</t>
+          <t>MLPClassifier IMBALANCE</t>
         </is>
       </c>
       <c r="B33" s="10" t="n">
-        <v>0.155</v>
+        <v>0.996</v>
       </c>
       <c r="C33" s="10" t="n">
-        <v>0.3769423558897243</v>
+        <v>0.4998745294855709</v>
       </c>
       <c r="D33" s="10" t="n">
-        <v>0.001774098166765228</v>
+        <v>0</v>
       </c>
       <c r="E33" s="10" t="n">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="F33" s="10" t="n">
-        <v>0.003537735849056603</v>
+        <v>0</v>
       </c>
       <c r="G33" s="10" t="n"/>
     </row>
     <row r="34">
       <c r="A34" s="10" t="inlineStr">
         <is>
-          <t>MLPClassifier IMBALANCE</t>
+          <t>MLPClassifier UNDERSAMPLE</t>
         </is>
       </c>
       <c r="B34" s="10" t="n">
-        <v>0.99675</v>
+        <v>0.9935</v>
       </c>
       <c r="C34" s="10" t="n">
-        <v>0.4997493106041614</v>
+        <v>0.4986198243412798</v>
       </c>
       <c r="D34" s="10" t="n">
         <v>0</v>
@@ -1572,14 +1572,14 @@
     <row r="35">
       <c r="A35" s="10" t="inlineStr">
         <is>
-          <t>KNN OVERSAMPLE</t>
+          <t>LR IMBALANCED</t>
         </is>
       </c>
       <c r="B35" s="10" t="n">
-        <v>0.9915</v>
+        <v>0.99625</v>
       </c>
       <c r="C35" s="10" t="n">
-        <v>0.4969924812030075</v>
+        <v>0.5</v>
       </c>
       <c r="D35" s="10" t="n">
         <v>0</v>
@@ -1595,11 +1595,11 @@
     <row r="36">
       <c r="A36" s="10" t="inlineStr">
         <is>
-          <t>LR IMBALANCED</t>
+          <t>LR UNDERSAMPLE</t>
         </is>
       </c>
       <c r="B36" s="10" t="n">
-        <v>0.99725</v>
+        <v>0.99625</v>
       </c>
       <c r="C36" s="10" t="n">
         <v>0.5</v>

</xml_diff>

<commit_message>
- Agregar setup.py - Agregar el guardado de los modelos DL - Arreglo de algunos detalles
</commit_message>
<xml_diff>
--- a/Experimentos.xlsx
+++ b/Experimentos.xlsx
@@ -538,37 +538,37 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="inlineStr">
+      <c r="A1" s="11" t="inlineStr">
         <is>
           <t>Test Size</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="11" t="inlineStr">
         <is>
           <t>Model</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="11" t="inlineStr">
         <is>
           <t>Accuracy</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" s="11" t="inlineStr">
         <is>
           <t>AUC</t>
         </is>
       </c>
-      <c r="E1" s="2" t="inlineStr">
+      <c r="E1" s="11" t="inlineStr">
         <is>
           <t>Precision Score</t>
         </is>
       </c>
-      <c r="F1" s="2" t="inlineStr">
+      <c r="F1" s="11" t="inlineStr">
         <is>
           <t>Recall Score</t>
         </is>
       </c>
-      <c r="G1" s="2" t="inlineStr">
+      <c r="G1" s="11" t="inlineStr">
         <is>
           <t>F1 Score</t>
         </is>
@@ -578,7 +578,7 @@
     </row>
     <row r="2">
       <c r="A2" s="10" t="n">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="B2" s="10" t="inlineStr">
         <is>
@@ -586,26 +586,26 @@
         </is>
       </c>
       <c r="C2" s="10" t="n">
-        <v>0.9966666666666667</v>
+        <v>0.99675</v>
       </c>
       <c r="D2" s="10" t="n">
-        <v>0.5238095238095238</v>
+        <v>0.5666666666666667</v>
       </c>
       <c r="E2" s="10" t="n">
         <v>1</v>
       </c>
       <c r="F2" s="10" t="n">
-        <v>0.04761904761904762</v>
+        <v>0.1333333333333333</v>
       </c>
       <c r="G2" s="10" t="n">
-        <v>0.0909090909090909</v>
+        <v>0.2352941176470588</v>
       </c>
       <c r="H2" s="10" t="n"/>
       <c r="I2" s="10" t="n"/>
     </row>
     <row r="3">
       <c r="A3" s="10" t="n">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="B3" s="10" t="inlineStr">
         <is>
@@ -613,26 +613,26 @@
         </is>
       </c>
       <c r="C3" s="10" t="n">
-        <v>0.9967</v>
+        <v>0.996</v>
       </c>
       <c r="D3" s="10" t="n">
-        <v>0.5147058823529411</v>
+        <v>0.5384615384615384</v>
       </c>
       <c r="E3" s="10" t="n">
         <v>1</v>
       </c>
       <c r="F3" s="10" t="n">
-        <v>0.02941176470588235</v>
+        <v>0.07692307692307693</v>
       </c>
       <c r="G3" s="10" t="n">
-        <v>0.05714285714285715</v>
+        <v>0.1428571428571429</v>
       </c>
       <c r="H3" s="10" t="n"/>
       <c r="I3" s="10" t="n"/>
     </row>
     <row r="4">
       <c r="A4" s="10" t="n">
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
       <c r="B4" s="10" t="inlineStr">
         <is>
@@ -640,26 +640,26 @@
         </is>
       </c>
       <c r="C4" s="10" t="n">
-        <v>0.996</v>
+        <v>0.9975000000000001</v>
       </c>
       <c r="D4" s="10" t="n">
-        <v>0.5</v>
+        <v>0.5238095238095238</v>
       </c>
       <c r="E4" s="10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4" s="10" t="n">
-        <v>0</v>
+        <v>0.04761904761904762</v>
       </c>
       <c r="G4" s="10" t="n">
-        <v>0</v>
+        <v>0.0909090909090909</v>
       </c>
       <c r="H4" s="10" t="n"/>
       <c r="I4" s="10" t="n"/>
     </row>
     <row r="5">
       <c r="A5" s="10" t="n">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="B5" s="10" t="inlineStr">
         <is>
@@ -667,26 +667,26 @@
         </is>
       </c>
       <c r="C5" s="10" t="n">
-        <v>0.99675</v>
+        <v>0.9974</v>
       </c>
       <c r="D5" s="10" t="n">
-        <v>0.5</v>
+        <v>0.5185185185185185</v>
       </c>
       <c r="E5" s="10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" s="10" t="n">
-        <v>0</v>
+        <v>0.03703703703703703</v>
       </c>
       <c r="G5" s="10" t="n">
-        <v>0</v>
+        <v>0.07142857142857142</v>
       </c>
       <c r="H5" s="10" t="n"/>
       <c r="I5" s="10" t="n"/>
     </row>
     <row r="6">
       <c r="A6" s="10" t="n">
-        <v>0.4</v>
+        <v>0.1</v>
       </c>
       <c r="B6" s="10" t="inlineStr">
         <is>

</xml_diff>